<commit_message>
small fixes - metal-sensing setting build to false - 2A peptides setting build to false - removing duplicates from build in CRISPR-Cas
</commit_message>
<xml_diff>
--- a/metal-sensing/metal-sensing.xlsx
+++ b/metal-sensing/metal-sensing.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d\Documents\GitHub\Forked_iGEM-distribution\metal-sensing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/metal-sensing/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40D9574-B128-D043-A373-51F7EC72E6D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="3045" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="-29380" yWindow="3020" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -23,18 +24,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Ontology Terms'!$A$1:$D$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -22727,7 +22717,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="24">
     <font>
       <sz val="12"/>
@@ -23077,7 +23067,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
@@ -23235,27 +23225,27 @@
     </dxf>
   </dxfs>
   <tableStyles count="5" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Basic Parts-style" pivot="0" count="3">
+    <tableStyle name="Basic Parts-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="headerRow" dxfId="16"/>
       <tableStyleElement type="firstRowStripe" dxfId="15"/>
       <tableStyleElement type="secondRowStripe" dxfId="14"/>
     </tableStyle>
-    <tableStyle name="Composite Parts-style" pivot="0" count="3">
+    <tableStyle name="Composite Parts-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="headerRow" dxfId="13"/>
       <tableStyleElement type="firstRowStripe" dxfId="12"/>
       <tableStyleElement type="secondRowStripe" dxfId="11"/>
     </tableStyle>
-    <tableStyle name="Composite Parts-style 2" pivot="0" count="3">
+    <tableStyle name="Composite Parts-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
       <tableStyleElement type="headerRow" dxfId="10"/>
       <tableStyleElement type="firstRowStripe" dxfId="9"/>
       <tableStyleElement type="secondRowStripe" dxfId="8"/>
     </tableStyle>
-    <tableStyle name="Composite Parts-style 3" pivot="0" count="3">
+    <tableStyle name="Composite Parts-style 3" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF03000000}">
       <tableStyleElement type="headerRow" dxfId="7"/>
       <tableStyleElement type="firstRowStripe" dxfId="6"/>
       <tableStyleElement type="secondRowStripe" dxfId="5"/>
     </tableStyle>
-    <tableStyle name="Composite Parts-style 4" pivot="0" count="3">
+    <tableStyle name="Composite Parts-style 4" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF04000000}">
       <tableStyleElement type="headerRow" dxfId="4"/>
       <tableStyleElement type="firstRowStripe" dxfId="3"/>
       <tableStyleElement type="secondRowStripe" dxfId="2"/>
@@ -23273,44 +23263,44 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A14:M39" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A14:M39" headerRowCount="0">
   <tableColumns count="13">
-    <tableColumn id="1" name="Column1"/>
-    <tableColumn id="2" name="Column2"/>
-    <tableColumn id="3" name="Column3"/>
-    <tableColumn id="4" name="Column4"/>
-    <tableColumn id="5" name="Column5"/>
-    <tableColumn id="6" name="Column6"/>
-    <tableColumn id="7" name="Column7"/>
-    <tableColumn id="8" name="Column8"/>
-    <tableColumn id="9" name="Column9"/>
-    <tableColumn id="10" name="Column10"/>
-    <tableColumn id="11" name="Column11"/>
-    <tableColumn id="12" name="Column12" dataDxfId="1"/>
-    <tableColumn id="13" name="Column13" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Column7"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Column9"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Column10"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column11"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Column12" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Column13" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium28" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_3" displayName="Table_3" ref="A13:O19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_3" displayName="Table_3" ref="A13:O19">
   <tableColumns count="15">
-    <tableColumn id="1" name="Part/Library Name"/>
-    <tableColumn id="2" name="Design Notes"/>
-    <tableColumn id="3" name="Part Description"/>
-    <tableColumn id="4" name="Final Product"/>
-    <tableColumn id="6" name="Backbone/locus"/>
-    <tableColumn id="7" name="Constraints"/>
-    <tableColumn id="8" name="Part 1"/>
-    <tableColumn id="9" name="Part 2"/>
-    <tableColumn id="10" name="Part 3"/>
-    <tableColumn id="11" name="Part 4"/>
-    <tableColumn id="12" name="Part 5"/>
-    <tableColumn id="13" name="Part 6"/>
-    <tableColumn id="14" name="Part 7"/>
-    <tableColumn id="15" name="Part 8"/>
-    <tableColumn id="16" name="Part 9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Part/Library Name"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Design Notes"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Part Description"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Final Product"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Backbone/locus"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Constraints"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Part 1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Part 2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Part 3"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Part 4"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="Part 5"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="Part 6"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="Part 7"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="Part 8"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="Part 9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium28" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -23513,27 +23503,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M963"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" style="14" customWidth="1"/>
-    <col min="3" max="3" width="42.33203125" style="14" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" style="14" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" style="14" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" style="14" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" style="14" customWidth="1"/>
-    <col min="9" max="9" width="15.5546875" style="14" customWidth="1"/>
-    <col min="10" max="11" width="8.44140625" style="14" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" style="14" customWidth="1"/>
-    <col min="13" max="13" width="34.44140625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="14" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" style="14" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" style="14" customWidth="1"/>
+    <col min="10" max="11" width="8.42578125" style="14" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="14" customWidth="1"/>
+    <col min="13" max="13" width="34.42578125" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1">
@@ -23608,7 +23598,7 @@
       <c r="L4" s="19"/>
       <c r="M4" s="19"/>
     </row>
-    <row r="5" spans="1:13" ht="45.95" customHeight="1">
+    <row r="5" spans="1:13" ht="46" customHeight="1">
       <c r="A5" s="45" t="s">
         <v>7552</v>
       </c>
@@ -25123,29 +25113,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.109375" style="14" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" style="14" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" style="14" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" style="14" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="14" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="14" customWidth="1"/>
     <col min="5" max="5" width="17" style="14" customWidth="1"/>
     <col min="6" max="6" width="15" style="14" customWidth="1"/>
-    <col min="7" max="12" width="20.88671875" style="14" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" style="14" customWidth="1"/>
-    <col min="14" max="15" width="8.6640625" style="14" customWidth="1"/>
-    <col min="16" max="16" width="17.109375" style="14" customWidth="1"/>
-    <col min="17" max="26" width="8.6640625" style="14" customWidth="1"/>
+    <col min="7" max="12" width="20.85546875" style="14" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" style="14" customWidth="1"/>
+    <col min="14" max="15" width="8.7109375" style="14" customWidth="1"/>
+    <col min="16" max="16" width="17.140625" style="14" customWidth="1"/>
+    <col min="17" max="26" width="8.7109375" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.95" customHeight="1">
+    <row r="1" spans="1:26" ht="16" customHeight="1">
       <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
@@ -25175,7 +25165,7 @@
       <c r="Y1" s="19"/>
       <c r="Z1" s="19"/>
     </row>
-    <row r="2" spans="1:26" ht="15.95" customHeight="1">
+    <row r="2" spans="1:26" ht="16" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -25205,7 +25195,7 @@
       <c r="Y2" s="19"/>
       <c r="Z2" s="19"/>
     </row>
-    <row r="3" spans="1:26" ht="15.95" customHeight="1">
+    <row r="3" spans="1:26" ht="16" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>50</v>
       </c>
@@ -25243,7 +25233,7 @@
       <c r="Y3" s="19"/>
       <c r="Z3" s="19"/>
     </row>
-    <row r="4" spans="1:26" ht="15.95" customHeight="1">
+    <row r="4" spans="1:26" ht="16" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>54</v>
       </c>
@@ -25283,7 +25273,7 @@
       <c r="Y4" s="19"/>
       <c r="Z4" s="19"/>
     </row>
-    <row r="5" spans="1:26" ht="15.95" customHeight="1">
+    <row r="5" spans="1:26" ht="16" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>59</v>
       </c>
@@ -25323,7 +25313,7 @@
       <c r="Y5" s="19"/>
       <c r="Z5" s="19"/>
     </row>
-    <row r="6" spans="1:26" ht="15.95" customHeight="1">
+    <row r="6" spans="1:26" ht="16" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>62</v>
       </c>
@@ -25359,7 +25349,7 @@
       <c r="Y6" s="19"/>
       <c r="Z6" s="19"/>
     </row>
-    <row r="7" spans="1:26" ht="15.95" customHeight="1">
+    <row r="7" spans="1:26" ht="16" customHeight="1">
       <c r="A7" s="6" t="s">
         <v>64</v>
       </c>
@@ -25403,7 +25393,7 @@
       <c r="Y7" s="19"/>
       <c r="Z7" s="19"/>
     </row>
-    <row r="8" spans="1:26" ht="15.95" customHeight="1">
+    <row r="8" spans="1:26" ht="16" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>67</v>
       </c>
@@ -25469,7 +25459,7 @@
       <c r="Y9" s="22"/>
       <c r="Z9" s="22"/>
     </row>
-    <row r="10" spans="1:26" ht="15.95" customHeight="1">
+    <row r="10" spans="1:26" ht="16" customHeight="1">
       <c r="A10" s="19"/>
       <c r="B10" s="19"/>
       <c r="C10" s="20" t="s">
@@ -25499,7 +25489,7 @@
       <c r="Y10" s="19"/>
       <c r="Z10" s="19"/>
     </row>
-    <row r="11" spans="1:26" ht="15.95" customHeight="1">
+    <row r="11" spans="1:26" ht="16" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>70</v>
       </c>
@@ -25642,7 +25632,7 @@
         <v>7535</v>
       </c>
       <c r="D14" s="19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="24" t="s">
         <v>48</v>
@@ -25671,7 +25661,7 @@
       <c r="Y14" s="19"/>
       <c r="Z14" s="19"/>
     </row>
-    <row r="15" spans="1:26" s="19" customFormat="1" ht="15.95" customHeight="1">
+    <row r="15" spans="1:26" s="19" customFormat="1" ht="16" customHeight="1">
       <c r="A15" s="43" t="s">
         <v>7534</v>
       </c>
@@ -25682,7 +25672,7 @@
         <v>7537</v>
       </c>
       <c r="D15" s="19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="24" t="s">
         <v>48</v>
@@ -25712,7 +25702,7 @@
         <v>7539</v>
       </c>
       <c r="D16" s="19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="24" t="s">
         <v>48</v>
@@ -25761,7 +25751,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
@@ -25769,11 +25759,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" style="14" customWidth="1"/>
     <col min="2" max="2" width="16" style="14" customWidth="1"/>
-    <col min="3" max="26" width="10.5546875" style="14" customWidth="1"/>
+    <col min="3" max="26" width="10.5703125" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1">
@@ -60656,13 +60646,13 @@
       <c r="C2535" s="30"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1"/>
+  <autoFilter ref="A1:D1" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <phoneticPr fontId="20"/>
   <hyperlinks>
-    <hyperlink ref="C752" r:id="rId1"/>
-    <hyperlink ref="C2371" r:id="rId2"/>
-    <hyperlink ref="C2372" r:id="rId3"/>
-    <hyperlink ref="C2518" r:id="rId4"/>
+    <hyperlink ref="C752" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="C2371" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="C2372" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="C2518" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -60670,7 +60660,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
@@ -60683,14 +60673,14 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="14" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="14" customWidth="1"/>
-    <col min="6" max="26" width="8.6640625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="14" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="14" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="14" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="14" customWidth="1"/>
+    <col min="6" max="26" width="8.7109375" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1">
@@ -61909,7 +61899,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
@@ -61919,9 +61909,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="26" width="8.6640625" style="14" customWidth="1"/>
+    <col min="1" max="26" width="8.7109375" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1">
@@ -63015,8 +63005,8 @@
   </sheetData>
   <phoneticPr fontId="20"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -63024,7 +63014,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
@@ -63032,14 +63022,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" style="14" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" style="14" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" style="14" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="14" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" style="14" customWidth="1"/>
-    <col min="6" max="26" width="8.6640625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="14" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="14" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" style="14" customWidth="1"/>
+    <col min="6" max="26" width="8.7109375" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1">
@@ -66259,33 +66249,33 @@
   </sheetData>
   <phoneticPr fontId="20"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="F2" r:id="rId3"/>
-    <hyperlink ref="C3" r:id="rId4"/>
-    <hyperlink ref="D3" r:id="rId5"/>
-    <hyperlink ref="F3" r:id="rId6"/>
-    <hyperlink ref="C4" r:id="rId7"/>
-    <hyperlink ref="D4" r:id="rId8"/>
-    <hyperlink ref="F4" r:id="rId9"/>
-    <hyperlink ref="C5" r:id="rId10"/>
-    <hyperlink ref="D5" r:id="rId11"/>
-    <hyperlink ref="F5" r:id="rId12"/>
-    <hyperlink ref="C6" r:id="rId13"/>
-    <hyperlink ref="D6" r:id="rId14"/>
-    <hyperlink ref="F6" r:id="rId15"/>
-    <hyperlink ref="C7" r:id="rId16"/>
-    <hyperlink ref="D7" r:id="rId17"/>
-    <hyperlink ref="F7" r:id="rId18"/>
-    <hyperlink ref="D8" r:id="rId19"/>
-    <hyperlink ref="F8" r:id="rId20" display="http://www.sevahub.es/public/Canonical/{REPLACE_HERE}/1"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="D3" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="F3" r:id="rId6" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="C4" r:id="rId7" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
+    <hyperlink ref="D4" r:id="rId8" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
+    <hyperlink ref="F4" r:id="rId9" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
+    <hyperlink ref="C5" r:id="rId10" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
+    <hyperlink ref="D5" r:id="rId11" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
+    <hyperlink ref="F5" r:id="rId12" xr:uid="{00000000-0004-0000-0500-00000B000000}"/>
+    <hyperlink ref="C6" r:id="rId13" xr:uid="{00000000-0004-0000-0500-00000C000000}"/>
+    <hyperlink ref="D6" r:id="rId14" xr:uid="{00000000-0004-0000-0500-00000D000000}"/>
+    <hyperlink ref="F6" r:id="rId15" xr:uid="{00000000-0004-0000-0500-00000E000000}"/>
+    <hyperlink ref="C7" r:id="rId16" xr:uid="{00000000-0004-0000-0500-00000F000000}"/>
+    <hyperlink ref="D7" r:id="rId17" xr:uid="{00000000-0004-0000-0500-000010000000}"/>
+    <hyperlink ref="F7" r:id="rId18" xr:uid="{00000000-0004-0000-0500-000011000000}"/>
+    <hyperlink ref="D8" r:id="rId19" xr:uid="{00000000-0004-0000-0500-000012000000}"/>
+    <hyperlink ref="F8" r:id="rId20" display="http://www.sevahub.es/public/Canonical/{REPLACE_HERE}/1" xr:uid="{00000000-0004-0000-0500-000013000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
@@ -66295,10 +66285,10 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" style="14" customWidth="1"/>
-    <col min="2" max="26" width="8.6640625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" style="14" customWidth="1"/>
+    <col min="2" max="26" width="8.7109375" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1">

</xml_diff>